<commit_message>
cambios en el trabajo practico nro2
</commit_message>
<xml_diff>
--- a/Trabajo práctico excel nro 3 B.xlsx
+++ b/Trabajo práctico excel nro 3 B.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alleg\Desktop\Curso de Excel y Word PDF\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alleg\Desktop\git carpeta nueva\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F8B72A-B5EC-459D-B631-70826C9147BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F770BDBD-1547-4C03-906F-C7432C4A6DF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" activeTab="1" xr2:uid="{269CABF4-E9E7-4CD9-BCF5-406FD890B13D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" activeTab="2" xr2:uid="{269CABF4-E9E7-4CD9-BCF5-406FD890B13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico1" sheetId="2" r:id="rId1"/>
@@ -566,28 +566,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>240</c:v>
+                  <c:v>680</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>360</c:v>
+                  <c:v>1020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>480</c:v>
+                  <c:v>1360</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>720</c:v>
+                  <c:v>2040</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>840</c:v>
+                  <c:v>2380</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>960</c:v>
+                  <c:v>2720</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -647,28 +647,28 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>270</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>390</c:v>
+                  <c:v>830</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>510</c:v>
+                  <c:v>1170</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>630</c:v>
+                  <c:v>1510</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>750</c:v>
+                  <c:v>1850</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>870</c:v>
+                  <c:v>2190</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>990</c:v>
+                  <c:v>2530</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1110</c:v>
+                  <c:v>2870</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1844,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D0C33B-C1C6-4DE7-8769-53E36CBDD5E2}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -2375,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CC762C-C76D-415C-BD87-FD672EC259A0}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" activeCellId="1" sqref="B1:K1 B3:K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,35 +2480,35 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>340</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>680</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="1"/>
-        <v>360</v>
+        <v>1020</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>1360</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>600</v>
+        <v>1700</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>720</v>
+        <v>2040</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="1"/>
-        <v>840</v>
+        <v>2380</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="1"/>
-        <v>960</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2521,35 +2521,35 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" ref="D5:K5" si="2">D3+D4</f>
-        <v>270</v>
+        <v>490</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="2"/>
-        <v>390</v>
+        <v>830</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="2"/>
-        <v>510</v>
+        <v>1170</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="2"/>
-        <v>630</v>
+        <v>1510</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="2"/>
-        <v>750</v>
+        <v>1850</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>870</v>
+        <v>2190</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="2"/>
-        <v>990</v>
+        <v>2530</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>1110</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2603,35 +2603,35 @@
       </c>
       <c r="D7" s="8">
         <f t="shared" ref="D7:K7" si="4">D6-D5</f>
-        <v>-120</v>
+        <v>-340</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" si="4"/>
-        <v>-90</v>
+        <v>-530</v>
       </c>
       <c r="F7" s="8">
         <f t="shared" si="4"/>
-        <v>-60</v>
+        <v>-720</v>
       </c>
       <c r="G7" s="8">
         <f t="shared" si="4"/>
-        <v>-30</v>
+        <v>-910</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-1100</v>
       </c>
       <c r="I7" s="8">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>-1290</v>
       </c>
       <c r="J7" s="8">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>-1480</v>
       </c>
       <c r="K7" s="8">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>-1670</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2658,7 +2658,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="1">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="C12" s="1">
         <f>C9/(C11-C10)</f>
-        <v>50</v>
+        <v>-7.8947368421052628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>